<commit_message>
PLAU Prod AU3 user fix
git-tfs-id: [https://dev.azure.com/TR-Legal-Cobalt]$/Cobalt QED Testing/PLPlusANZ;C1213074
</commit_message>
<xml_diff>
--- a/PLPlusANZ-Tests/src/test/resources/CobaltUsers.xlsx
+++ b/PLPlusANZ-Tests/src/test/resources/CobaltUsers.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23127"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D404EA94-3ADA-4111-8925-B88544AB7F53}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C82BABFD-4EC8-4A5C-BC2B-CFA6828E1CCA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="10440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -391,7 +391,7 @@
     <t>P@ssword2</t>
   </si>
   <si>
-    <t>P@ssword3</t>
+    <t>P@ssword4</t>
   </si>
 </sst>
 </file>
@@ -852,7 +852,7 @@
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A13" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="C22" sqref="C22"/>
+      <selection pane="topRight" activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
PLAU Folders suite rebalancing
git-tfs-id: [https://dev.azure.com/TR-Legal-Cobalt]$/Cobalt QED Testing/PLPlusANZ;C1213668
</commit_message>
<xml_diff>
--- a/PLPlusANZ-Tests/src/test/resources/CobaltUsers.xlsx
+++ b/PLPlusANZ-Tests/src/test/resources/CobaltUsers.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23127"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C82BABFD-4EC8-4A5C-BC2B-CFA6828E1CCA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FAF16FB5-759A-4D71-A658-4D8116672679}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="10440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="126">
   <si>
     <t>UserName</t>
   </si>
@@ -392,6 +392,12 @@
   </si>
   <si>
     <t>P@ssword4</t>
+  </si>
+  <si>
+    <t>PLANZtestuser2</t>
+  </si>
+  <si>
+    <t>PLANZtestuser2@mailinator.com</t>
   </si>
 </sst>
 </file>
@@ -437,7 +443,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -486,12 +492,23 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -499,7 +516,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="1" applyBorder="1"/>
@@ -509,6 +525,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -850,9 +868,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="C19" sqref="C19"/>
+      <selection pane="topRight" activeCell="D32" sqref="D32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -889,7 +907,7 @@
       <c r="F1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="G1" s="8" t="s">
+      <c r="G1" s="7" t="s">
         <v>14</v>
       </c>
       <c r="H1" s="1" t="s">
@@ -927,7 +945,7 @@
       <c r="F2" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="G2" s="9" t="s">
+      <c r="G2" s="8" t="s">
         <v>31</v>
       </c>
       <c r="H2" s="4"/>
@@ -953,7 +971,7 @@
       <c r="F3" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="G3" s="10" t="s">
+      <c r="G3" s="9" t="s">
         <v>18</v>
       </c>
       <c r="H3" s="5"/>
@@ -963,7 +981,7 @@
       <c r="L3" s="4"/>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A4" s="12" t="s">
+      <c r="A4" s="11" t="s">
         <v>17</v>
       </c>
       <c r="B4" s="5" t="s">
@@ -977,12 +995,12 @@
       <c r="F4" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="G4" s="11" t="s">
+      <c r="G4" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="H4" s="12"/>
-      <c r="I4" s="15"/>
-      <c r="J4" s="12" t="s">
+      <c r="H4" s="11"/>
+      <c r="I4" s="14"/>
+      <c r="J4" s="11" t="s">
         <v>94</v>
       </c>
       <c r="K4" s="5" t="s">
@@ -1005,12 +1023,12 @@
       <c r="F5" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="G5" s="10" t="s">
+      <c r="G5" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="H5" s="12"/>
+      <c r="H5" s="11"/>
       <c r="I5" s="5"/>
-      <c r="J5" s="12"/>
+      <c r="J5" s="11"/>
       <c r="K5" s="5"/>
       <c r="L5" s="4"/>
     </row>
@@ -1029,12 +1047,12 @@
       <c r="F6" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="G6" s="10" t="s">
+      <c r="G6" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="H6" s="12"/>
+      <c r="H6" s="11"/>
       <c r="I6" s="5"/>
-      <c r="J6" s="12"/>
+      <c r="J6" s="11"/>
       <c r="K6" s="5"/>
       <c r="L6" s="4"/>
     </row>
@@ -1053,12 +1071,12 @@
       <c r="F7" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="G7" s="10" t="s">
+      <c r="G7" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="H7" s="12"/>
+      <c r="H7" s="11"/>
       <c r="I7" s="5"/>
-      <c r="J7" s="12"/>
+      <c r="J7" s="11"/>
       <c r="K7" s="5"/>
       <c r="L7" s="4"/>
     </row>
@@ -1073,12 +1091,12 @@
       <c r="D8" s="4"/>
       <c r="E8" s="4"/>
       <c r="F8" s="4"/>
-      <c r="G8" s="9" t="s">
+      <c r="G8" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="H8" s="12"/>
+      <c r="H8" s="11"/>
       <c r="I8" s="4"/>
-      <c r="J8" s="12"/>
+      <c r="J8" s="11"/>
       <c r="K8" s="4"/>
       <c r="L8" s="4"/>
     </row>
@@ -1093,12 +1111,12 @@
       <c r="D9" s="4"/>
       <c r="E9" s="4"/>
       <c r="F9" s="4"/>
-      <c r="G9" s="9" t="s">
+      <c r="G9" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="H9" s="12"/>
+      <c r="H9" s="11"/>
       <c r="I9" s="4"/>
-      <c r="J9" s="12"/>
+      <c r="J9" s="11"/>
       <c r="K9" s="4"/>
       <c r="L9" s="4"/>
     </row>
@@ -1117,10 +1135,10 @@
       <c r="F10" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="G10" s="9"/>
-      <c r="H10" s="12"/>
+      <c r="G10" s="8"/>
+      <c r="H10" s="11"/>
       <c r="I10" s="4"/>
-      <c r="J10" s="12"/>
+      <c r="J10" s="11"/>
       <c r="K10" s="4"/>
       <c r="L10" s="4"/>
     </row>
@@ -1139,10 +1157,10 @@
       <c r="F11" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="G11" s="9"/>
-      <c r="H11" s="12"/>
+      <c r="G11" s="8"/>
+      <c r="H11" s="11"/>
       <c r="I11" s="4"/>
-      <c r="J11" s="12"/>
+      <c r="J11" s="11"/>
       <c r="K11" s="4"/>
       <c r="L11" s="4"/>
     </row>
@@ -1165,10 +1183,10 @@
       <c r="F12" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="G12" s="9"/>
-      <c r="H12" s="12"/>
+      <c r="G12" s="8"/>
+      <c r="H12" s="11"/>
       <c r="I12" s="4"/>
-      <c r="J12" s="12"/>
+      <c r="J12" s="11"/>
       <c r="K12" s="4"/>
       <c r="L12" s="4"/>
     </row>
@@ -1191,15 +1209,15 @@
       <c r="F13" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="G13" s="9"/>
-      <c r="H13" s="12"/>
+      <c r="G13" s="8"/>
+      <c r="H13" s="11"/>
       <c r="I13" s="4"/>
-      <c r="J13" s="12"/>
+      <c r="J13" s="11"/>
       <c r="K13" s="4"/>
       <c r="L13" s="4"/>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A14" s="12" t="s">
+      <c r="A14" s="11" t="s">
         <v>57</v>
       </c>
       <c r="B14" s="4" t="s">
@@ -1211,19 +1229,19 @@
       </c>
       <c r="E14" s="4"/>
       <c r="F14" s="4"/>
-      <c r="G14" s="10" t="s">
+      <c r="G14" s="9" t="s">
         <v>58</v>
       </c>
-      <c r="H14" s="12"/>
+      <c r="H14" s="11"/>
       <c r="I14" s="5"/>
-      <c r="J14" s="12"/>
+      <c r="J14" s="11"/>
       <c r="K14" s="5"/>
       <c r="L14" s="4" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A15" s="12" t="s">
+      <c r="A15" s="11" t="s">
         <v>60</v>
       </c>
       <c r="B15" s="5" t="s">
@@ -1235,12 +1253,12 @@
       </c>
       <c r="E15" s="4"/>
       <c r="F15" s="4"/>
-      <c r="G15" s="10" t="s">
+      <c r="G15" s="9" t="s">
         <v>59</v>
       </c>
-      <c r="H15" s="12"/>
-      <c r="I15" s="16"/>
-      <c r="J15" s="12" t="s">
+      <c r="H15" s="11"/>
+      <c r="I15" s="15"/>
+      <c r="J15" s="11" t="s">
         <v>95</v>
       </c>
       <c r="K15" s="5" t="s">
@@ -1251,7 +1269,7 @@
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A16" s="12" t="s">
+      <c r="A16" s="11" t="s">
         <v>62</v>
       </c>
       <c r="B16" s="5" t="s">
@@ -1261,11 +1279,11 @@
       <c r="D16" s="4"/>
       <c r="E16" s="4"/>
       <c r="F16" s="4"/>
-      <c r="G16" s="10" t="s">
+      <c r="G16" s="9" t="s">
         <v>61</v>
       </c>
       <c r="H16" s="2"/>
-      <c r="I16" s="16"/>
+      <c r="I16" s="15"/>
       <c r="J16" s="2" t="s">
         <v>96</v>
       </c>
@@ -1277,7 +1295,7 @@
       </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A17" s="12" t="s">
+      <c r="A17" s="11" t="s">
         <v>66</v>
       </c>
       <c r="B17" s="5" t="s">
@@ -1287,11 +1305,11 @@
       <c r="D17" s="4"/>
       <c r="E17" s="4"/>
       <c r="F17" s="4"/>
-      <c r="G17" s="10" t="s">
+      <c r="G17" s="9" t="s">
         <v>65</v>
       </c>
       <c r="H17" s="2"/>
-      <c r="I17" s="16"/>
+      <c r="I17" s="15"/>
       <c r="J17" s="2" t="s">
         <v>97</v>
       </c>
@@ -1303,7 +1321,7 @@
       </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A18" s="12" t="s">
+      <c r="A18" s="11" t="s">
         <v>67</v>
       </c>
       <c r="B18" s="5" t="s">
@@ -1313,7 +1331,7 @@
       <c r="D18" s="4"/>
       <c r="E18" s="4"/>
       <c r="F18" s="4"/>
-      <c r="G18" s="10" t="s">
+      <c r="G18" s="9" t="s">
         <v>68</v>
       </c>
       <c r="H18" s="5"/>
@@ -1329,7 +1347,7 @@
       </c>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A19" s="12" t="s">
+      <c r="A19" s="11" t="s">
         <v>70</v>
       </c>
       <c r="B19" s="5" t="s">
@@ -1339,7 +1357,7 @@
       <c r="D19" s="4"/>
       <c r="E19" s="4"/>
       <c r="F19" s="4"/>
-      <c r="G19" s="10" t="s">
+      <c r="G19" s="9" t="s">
         <v>71</v>
       </c>
       <c r="H19" s="5"/>
@@ -1355,7 +1373,7 @@
       </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A20" s="12" t="s">
+      <c r="A20" s="11" t="s">
         <v>72</v>
       </c>
       <c r="B20" s="5" t="s">
@@ -1365,7 +1383,7 @@
       <c r="D20" s="4"/>
       <c r="E20" s="4"/>
       <c r="F20" s="4"/>
-      <c r="G20" s="10" t="s">
+      <c r="G20" s="9" t="s">
         <v>73</v>
       </c>
       <c r="H20" s="5"/>
@@ -1381,7 +1399,7 @@
       </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A21" s="12" t="s">
+      <c r="A21" s="11" t="s">
         <v>74</v>
       </c>
       <c r="B21" s="5" t="s">
@@ -1391,7 +1409,7 @@
       <c r="D21" s="4"/>
       <c r="E21" s="4"/>
       <c r="F21" s="4"/>
-      <c r="G21" s="10" t="s">
+      <c r="G21" s="9" t="s">
         <v>75</v>
       </c>
       <c r="H21" s="5"/>
@@ -1407,7 +1425,7 @@
       </c>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A22" s="12" t="s">
+      <c r="A22" s="11" t="s">
         <v>76</v>
       </c>
       <c r="B22" s="5" t="s">
@@ -1417,7 +1435,7 @@
       <c r="D22" s="4"/>
       <c r="E22" s="4"/>
       <c r="F22" s="4"/>
-      <c r="G22" s="10" t="s">
+      <c r="G22" s="9" t="s">
         <v>77</v>
       </c>
       <c r="H22" s="5"/>
@@ -1433,7 +1451,7 @@
       </c>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A23" s="12" t="s">
+      <c r="A23" s="11" t="s">
         <v>78</v>
       </c>
       <c r="B23" s="5" t="s">
@@ -1443,7 +1461,7 @@
       <c r="D23" s="4"/>
       <c r="E23" s="4"/>
       <c r="F23" s="4"/>
-      <c r="G23" s="10" t="s">
+      <c r="G23" s="9" t="s">
         <v>79</v>
       </c>
       <c r="H23" s="5"/>
@@ -1459,7 +1477,7 @@
       </c>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A24" s="12" t="s">
+      <c r="A24" s="11" t="s">
         <v>80</v>
       </c>
       <c r="B24" s="4" t="s">
@@ -1469,7 +1487,7 @@
       <c r="D24" s="4"/>
       <c r="E24" s="4"/>
       <c r="F24" s="4"/>
-      <c r="G24" s="10" t="s">
+      <c r="G24" s="9" t="s">
         <v>81</v>
       </c>
       <c r="H24" s="5"/>
@@ -1481,7 +1499,7 @@
       </c>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A25" s="12" t="s">
+      <c r="A25" s="11" t="s">
         <v>82</v>
       </c>
       <c r="B25" s="4" t="s">
@@ -1491,7 +1509,7 @@
       <c r="D25" s="4"/>
       <c r="E25" s="4"/>
       <c r="F25" s="4"/>
-      <c r="G25" s="10" t="s">
+      <c r="G25" s="9" t="s">
         <v>83</v>
       </c>
       <c r="H25" s="5"/>
@@ -1503,7 +1521,7 @@
       </c>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A26" s="12" t="s">
+      <c r="A26" s="11" t="s">
         <v>84</v>
       </c>
       <c r="B26" s="5" t="s">
@@ -1513,7 +1531,7 @@
       <c r="D26" s="4"/>
       <c r="E26" s="4"/>
       <c r="F26" s="4"/>
-      <c r="G26" s="10" t="s">
+      <c r="G26" s="9" t="s">
         <v>87</v>
       </c>
       <c r="H26" s="5"/>
@@ -1529,7 +1547,7 @@
       </c>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A27" s="12" t="s">
+      <c r="A27" s="11" t="s">
         <v>85</v>
       </c>
       <c r="B27" s="5" t="s">
@@ -1539,7 +1557,7 @@
       <c r="D27" s="4"/>
       <c r="E27" s="4"/>
       <c r="F27" s="4"/>
-      <c r="G27" s="10" t="s">
+      <c r="G27" s="9" t="s">
         <v>86</v>
       </c>
       <c r="H27" s="5"/>
@@ -1565,7 +1583,7 @@
       <c r="D28" s="4"/>
       <c r="E28" s="4"/>
       <c r="F28" s="4"/>
-      <c r="G28" s="10" t="s">
+      <c r="G28" s="9" t="s">
         <v>89</v>
       </c>
       <c r="H28" s="5"/>
@@ -1589,7 +1607,7 @@
         <v>45</v>
       </c>
       <c r="F29" s="4"/>
-      <c r="G29" s="9" t="s">
+      <c r="G29" s="8" t="s">
         <v>46</v>
       </c>
       <c r="H29" s="4"/>
@@ -1615,7 +1633,7 @@
         <v>45</v>
       </c>
       <c r="F30" s="4"/>
-      <c r="G30" s="10" t="s">
+      <c r="G30" s="9" t="s">
         <v>55</v>
       </c>
       <c r="H30" s="5"/>
@@ -1641,7 +1659,7 @@
         <v>45</v>
       </c>
       <c r="F31" s="4"/>
-      <c r="G31" s="10" t="s">
+      <c r="G31" s="9" t="s">
         <v>56</v>
       </c>
       <c r="H31" s="5"/>
@@ -1663,7 +1681,7 @@
         <v>45</v>
       </c>
       <c r="F32" s="4"/>
-      <c r="G32" s="10" t="s">
+      <c r="G32" s="9" t="s">
         <v>48</v>
       </c>
       <c r="H32" s="5"/>
@@ -1685,7 +1703,7 @@
         <v>45</v>
       </c>
       <c r="F33" s="4"/>
-      <c r="G33" s="10" t="s">
+      <c r="G33" s="9" t="s">
         <v>50</v>
       </c>
       <c r="H33" s="5"/>
@@ -1695,33 +1713,46 @@
       <c r="L33" s="4"/>
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A34" s="2" t="s">
+      <c r="A34" s="16" t="s">
         <v>51</v>
       </c>
-      <c r="B34" s="4" t="s">
+      <c r="B34" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="C34" s="4"/>
-      <c r="D34" s="4"/>
-      <c r="E34" s="4" t="s">
+      <c r="C34" s="13"/>
+      <c r="D34" s="13"/>
+      <c r="E34" s="13" t="s">
         <v>45</v>
       </c>
-      <c r="F34" s="4"/>
-      <c r="G34" s="10" t="s">
+      <c r="F34" s="13"/>
+      <c r="G34" s="17" t="s">
         <v>52</v>
       </c>
-      <c r="H34" s="13"/>
-      <c r="I34" s="13"/>
-      <c r="J34" s="13"/>
-      <c r="K34" s="13"/>
-      <c r="L34" s="14"/>
+      <c r="H34" s="12"/>
+      <c r="I34" s="12"/>
+      <c r="J34" s="12"/>
+      <c r="K34" s="12"/>
+      <c r="L34" s="13"/>
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="H35" s="7"/>
-      <c r="I35" s="7"/>
-      <c r="J35" s="7"/>
-      <c r="K35" s="7"/>
-      <c r="L35" s="7"/>
+      <c r="A35" s="4" t="s">
+        <v>124</v>
+      </c>
+      <c r="B35" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="C35" s="4"/>
+      <c r="D35" s="4"/>
+      <c r="E35" s="4"/>
+      <c r="F35" s="4"/>
+      <c r="G35" s="5" t="s">
+        <v>125</v>
+      </c>
+      <c r="H35" s="4"/>
+      <c r="I35" s="4"/>
+      <c r="J35" s="4"/>
+      <c r="K35" s="4"/>
+      <c r="L35" s="4"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:L34" xr:uid="{46BB54A7-56CE-4320-A2E8-912A1AFF98E7}"/>
@@ -1780,9 +1811,11 @@
     <hyperlink ref="B26" r:id="rId52" xr:uid="{5A9A556E-193D-4906-BD07-952EF6BF8A37}"/>
     <hyperlink ref="B29" r:id="rId53" xr:uid="{DBE6C47B-31D5-4908-8C16-D56DABF274BE}"/>
     <hyperlink ref="B30" r:id="rId54" xr:uid="{3812BCE2-3A74-426B-B41D-3AFE6E7BDADB}"/>
+    <hyperlink ref="B35" r:id="rId55" xr:uid="{F9CEA64B-443C-4110-8FE5-4820AD15E535}"/>
+    <hyperlink ref="G35" r:id="rId56" xr:uid="{AF615813-6EF6-4298-A920-CB3FCA725BE7}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId55"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId57"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
PLAU Login suite rebalancing
git-tfs-id: [https://dev.azure.com/TR-Legal-Cobalt]$/Cobalt QED Testing/PLPlusANZ;C1214274
</commit_message>
<xml_diff>
--- a/PLPlusANZ-Tests/src/test/resources/CobaltUsers.xlsx
+++ b/PLPlusANZ-Tests/src/test/resources/CobaltUsers.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23127"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FAF16FB5-759A-4D71-A658-4D8116672679}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E16D8A8-4678-465F-A9C7-407731099EEE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="10440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="129">
   <si>
     <t>UserName</t>
   </si>
@@ -398,6 +398,15 @@
   </si>
   <si>
     <t>PLANZtestuser2@mailinator.com</t>
+  </si>
+  <si>
+    <t>PLAUtestuser14</t>
+  </si>
+  <si>
+    <t>PLAUtestuser14@mailinator.com</t>
+  </si>
+  <si>
+    <t>PLAUtestuser13</t>
   </si>
 </sst>
 </file>
@@ -866,11 +875,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L35"/>
+  <dimension ref="A1:L37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="D32" sqref="D32"/>
+      <selection pane="topRight" activeCell="D42" sqref="D42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1753,6 +1762,52 @@
       <c r="J35" s="4"/>
       <c r="K35" s="4"/>
       <c r="L35" s="4"/>
+    </row>
+    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A36" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="B36" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="C36" s="4"/>
+      <c r="D36" s="4"/>
+      <c r="E36" s="4"/>
+      <c r="F36" s="4"/>
+      <c r="G36" s="5" t="s">
+        <v>127</v>
+      </c>
+      <c r="H36" s="4"/>
+      <c r="I36" s="4"/>
+      <c r="J36" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="K36" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="L36" s="4"/>
+    </row>
+    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A37" s="4" t="s">
+        <v>128</v>
+      </c>
+      <c r="B37" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="C37" s="4"/>
+      <c r="D37" s="4"/>
+      <c r="E37" s="4"/>
+      <c r="F37" s="4"/>
+      <c r="G37" s="4"/>
+      <c r="H37" s="4"/>
+      <c r="I37" s="4"/>
+      <c r="J37" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="K37" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="L37" s="4"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:L34" xr:uid="{46BB54A7-56CE-4320-A2E8-912A1AFF98E7}"/>
@@ -1813,9 +1868,14 @@
     <hyperlink ref="B30" r:id="rId54" xr:uid="{3812BCE2-3A74-426B-B41D-3AFE6E7BDADB}"/>
     <hyperlink ref="B35" r:id="rId55" xr:uid="{F9CEA64B-443C-4110-8FE5-4820AD15E535}"/>
     <hyperlink ref="G35" r:id="rId56" xr:uid="{AF615813-6EF6-4298-A920-CB3FCA725BE7}"/>
+    <hyperlink ref="G36" r:id="rId57" xr:uid="{02DDA79B-6CBE-41EA-84CE-F4410C4C1ED3}"/>
+    <hyperlink ref="B36" r:id="rId58" xr:uid="{3B40A8B7-5C95-4E55-8B4F-B41B13B7D3E8}"/>
+    <hyperlink ref="B37" r:id="rId59" xr:uid="{6D6C1314-AAE2-43C6-887C-45E123CE73D9}"/>
+    <hyperlink ref="K36" r:id="rId60" xr:uid="{A52B8DEE-94FA-485F-93A1-69AF321E3109}"/>
+    <hyperlink ref="K37" r:id="rId61" xr:uid="{D5BA73F5-B19B-47F9-AB06-4D1B19B21204}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId57"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId62"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
PLAu BreadCrumb suite rebalancing
git-tfs-id: [https://dev.azure.com/TR-Legal-Cobalt]$/Cobalt QED Testing/PLPlusANZ;C1214280
</commit_message>
<xml_diff>
--- a/PLPlusANZ-Tests/src/test/resources/CobaltUsers.xlsx
+++ b/PLPlusANZ-Tests/src/test/resources/CobaltUsers.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23127"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E16D8A8-4678-465F-A9C7-407731099EEE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6BDA035-C842-495A-9C62-41A9A8E43177}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="10440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="138">
   <si>
     <t>UserName</t>
   </si>
@@ -400,13 +400,40 @@
     <t>PLANZtestuser2@mailinator.com</t>
   </si>
   <si>
+    <t>PLAUtestuser1</t>
+  </si>
+  <si>
+    <t>PLAUtestuser2</t>
+  </si>
+  <si>
     <t>PLAUtestuser14</t>
   </si>
   <si>
+    <t>PLAUtestuser13</t>
+  </si>
+  <si>
     <t>PLAUtestuser14@mailinator.com</t>
   </si>
   <si>
-    <t>PLAUtestuser13</t>
+    <t>PLAUtestuser13@mailinator.com</t>
+  </si>
+  <si>
+    <t>PLAUtestuser1@mailinator.com</t>
+  </si>
+  <si>
+    <t>PLAUtestuser2@mailinator.com</t>
+  </si>
+  <si>
+    <t>PLAUtestuser3</t>
+  </si>
+  <si>
+    <t>PLAUtestuser4</t>
+  </si>
+  <si>
+    <t>PLAUtestuser3@mailinator.com</t>
+  </si>
+  <si>
+    <t>PLAUtestuser4@mailinator.com</t>
   </si>
 </sst>
 </file>
@@ -875,11 +902,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L37"/>
+  <dimension ref="A1:L41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A23" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="D42" sqref="D42"/>
+      <selection pane="topRight" activeCell="C43" sqref="C43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1765,7 +1792,7 @@
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A36" s="4" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="B36" s="5" t="s">
         <v>122</v>
@@ -1775,7 +1802,7 @@
       <c r="E36" s="4"/>
       <c r="F36" s="4"/>
       <c r="G36" s="5" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
       <c r="H36" s="4"/>
       <c r="I36" s="4"/>
@@ -1785,11 +1812,13 @@
       <c r="K36" s="5" t="s">
         <v>119</v>
       </c>
-      <c r="L36" s="4"/>
+      <c r="L36" s="4" t="s">
+        <v>63</v>
+      </c>
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A37" s="4" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="B37" s="5" t="s">
         <v>122</v>
@@ -1798,7 +1827,9 @@
       <c r="D37" s="4"/>
       <c r="E37" s="4"/>
       <c r="F37" s="4"/>
-      <c r="G37" s="4"/>
+      <c r="G37" s="5" t="s">
+        <v>131</v>
+      </c>
       <c r="H37" s="4"/>
       <c r="I37" s="4"/>
       <c r="J37" s="2" t="s">
@@ -1807,7 +1838,109 @@
       <c r="K37" s="5" t="s">
         <v>119</v>
       </c>
-      <c r="L37" s="4"/>
+      <c r="L37" s="4" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A38" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="B38" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="C38" s="4"/>
+      <c r="D38" s="4"/>
+      <c r="E38" s="4"/>
+      <c r="F38" s="4"/>
+      <c r="G38" s="5" t="s">
+        <v>132</v>
+      </c>
+      <c r="H38" s="4"/>
+      <c r="I38" s="4"/>
+      <c r="J38" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="K38" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="L38" s="4"/>
+    </row>
+    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A39" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="B39" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="C39" s="4"/>
+      <c r="D39" s="4"/>
+      <c r="E39" s="4"/>
+      <c r="F39" s="4"/>
+      <c r="G39" s="5" t="s">
+        <v>133</v>
+      </c>
+      <c r="H39" s="4"/>
+      <c r="I39" s="4"/>
+      <c r="J39" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="K39" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="L39" s="4"/>
+    </row>
+    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A40" s="4" t="s">
+        <v>134</v>
+      </c>
+      <c r="B40" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="C40" s="4"/>
+      <c r="D40" s="4"/>
+      <c r="E40" s="4"/>
+      <c r="F40" s="4"/>
+      <c r="G40" s="5" t="s">
+        <v>136</v>
+      </c>
+      <c r="H40" s="4"/>
+      <c r="I40" s="4"/>
+      <c r="J40" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="K40" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="L40" s="4" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A41" s="4" t="s">
+        <v>135</v>
+      </c>
+      <c r="B41" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="C41" s="4"/>
+      <c r="D41" s="4"/>
+      <c r="E41" s="4"/>
+      <c r="F41" s="4"/>
+      <c r="G41" s="5" t="s">
+        <v>137</v>
+      </c>
+      <c r="H41" s="4"/>
+      <c r="I41" s="4"/>
+      <c r="J41" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="K41" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="L41" s="4" t="s">
+        <v>63</v>
+      </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:L34" xr:uid="{46BB54A7-56CE-4320-A2E8-912A1AFF98E7}"/>
@@ -1868,14 +2001,26 @@
     <hyperlink ref="B30" r:id="rId54" xr:uid="{3812BCE2-3A74-426B-B41D-3AFE6E7BDADB}"/>
     <hyperlink ref="B35" r:id="rId55" xr:uid="{F9CEA64B-443C-4110-8FE5-4820AD15E535}"/>
     <hyperlink ref="G35" r:id="rId56" xr:uid="{AF615813-6EF6-4298-A920-CB3FCA725BE7}"/>
-    <hyperlink ref="G36" r:id="rId57" xr:uid="{02DDA79B-6CBE-41EA-84CE-F4410C4C1ED3}"/>
-    <hyperlink ref="B36" r:id="rId58" xr:uid="{3B40A8B7-5C95-4E55-8B4F-B41B13B7D3E8}"/>
-    <hyperlink ref="B37" r:id="rId59" xr:uid="{6D6C1314-AAE2-43C6-887C-45E123CE73D9}"/>
-    <hyperlink ref="K36" r:id="rId60" xr:uid="{A52B8DEE-94FA-485F-93A1-69AF321E3109}"/>
-    <hyperlink ref="K37" r:id="rId61" xr:uid="{D5BA73F5-B19B-47F9-AB06-4D1B19B21204}"/>
+    <hyperlink ref="B38" r:id="rId57" xr:uid="{89F25A13-A172-497F-8CE3-5D4409F41B4F}"/>
+    <hyperlink ref="B39" r:id="rId58" xr:uid="{24E87864-B135-49BA-BE62-962A47FCE58C}"/>
+    <hyperlink ref="K38" r:id="rId59" xr:uid="{40477EF3-2B66-4270-8235-D256CBAB4BBF}"/>
+    <hyperlink ref="K39" r:id="rId60" xr:uid="{BAD7E65A-8416-4F76-AE1C-2B21061C4463}"/>
+    <hyperlink ref="B36" r:id="rId61" xr:uid="{6D23639B-B2F3-48A4-A5D8-C0C4999D4D92}"/>
+    <hyperlink ref="K36" r:id="rId62" xr:uid="{4586EFD4-4608-4D09-9B23-192D12EE1FDF}"/>
+    <hyperlink ref="K37" r:id="rId63" xr:uid="{F37A5A5A-E6D6-45C7-9B40-0E4C7A81FDF0}"/>
+    <hyperlink ref="G36" r:id="rId64" xr:uid="{044F65C8-9B95-454E-8FD5-518DDDB9FB9B}"/>
+    <hyperlink ref="G37" r:id="rId65" xr:uid="{C953582D-F248-41C5-AC5B-A2EFB1FDA5EB}"/>
+    <hyperlink ref="G38" r:id="rId66" xr:uid="{6BC6EE1B-7E5F-4759-AA23-CEFF794BE365}"/>
+    <hyperlink ref="G39" r:id="rId67" xr:uid="{FA510CBE-0B1E-4C43-83D2-CE5F63427358}"/>
+    <hyperlink ref="B40" r:id="rId68" xr:uid="{E30FCD2F-28D5-472A-828D-370C1C5BEB7E}"/>
+    <hyperlink ref="B41" r:id="rId69" xr:uid="{F1B8F9CA-7DE9-46CE-BBA1-E7553E7DCDB1}"/>
+    <hyperlink ref="G40" r:id="rId70" xr:uid="{92DBAF28-DCED-4F04-BECB-34A8DC3BA4C5}"/>
+    <hyperlink ref="G41" r:id="rId71" xr:uid="{2E0446EE-618A-454A-9D8B-4B27BD2F86DA}"/>
+    <hyperlink ref="K40" r:id="rId72" xr:uid="{16F44302-BF74-4A5B-90C5-1E10BF88A0E2}"/>
+    <hyperlink ref="K41" r:id="rId73" xr:uid="{0740A5E4-8C6B-4E30-A1C1-E1D4E4DE7981}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId62"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId74"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
PLAU pagination xpath fix
git-tfs-id: [https://dev.azure.com/TR-Legal-Cobalt]$/Cobalt QED Testing/PLPlusANZ;C1218116
</commit_message>
<xml_diff>
--- a/PLPlusANZ-Tests/src/test/resources/CobaltUsers.xlsx
+++ b/PLPlusANZ-Tests/src/test/resources/CobaltUsers.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23127"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6BDA035-C842-495A-9C62-41A9A8E43177}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F525FF6-7CC7-4DAE-A05A-760356C8F6FB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="10440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="138">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="140">
   <si>
     <t>UserName</t>
   </si>
@@ -434,6 +434,12 @@
   </si>
   <si>
     <t>PLAUtestuser4@mailinator.com</t>
+  </si>
+  <si>
+    <t>PLNewAUtestuser4</t>
+  </si>
+  <si>
+    <t>PLNewAUtestuser4@mailinator.com</t>
   </si>
 </sst>
 </file>
@@ -902,11 +908,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L41"/>
+  <dimension ref="A1:L42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="C43" sqref="C43"/>
+    <sheetView tabSelected="1" topLeftCell="A33" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="F1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="H50" sqref="H50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1939,6 +1945,32 @@
         <v>110</v>
       </c>
       <c r="L41" s="4" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A42" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="B42" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="C42" s="4"/>
+      <c r="D42" s="4"/>
+      <c r="E42" s="4"/>
+      <c r="F42" s="4"/>
+      <c r="G42" s="5" t="s">
+        <v>139</v>
+      </c>
+      <c r="H42" s="4"/>
+      <c r="I42" s="4"/>
+      <c r="J42" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="K42" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="L42" s="4" t="s">
         <v>63</v>
       </c>
     </row>
@@ -2018,9 +2050,11 @@
     <hyperlink ref="G41" r:id="rId71" xr:uid="{2E0446EE-618A-454A-9D8B-4B27BD2F86DA}"/>
     <hyperlink ref="K40" r:id="rId72" xr:uid="{16F44302-BF74-4A5B-90C5-1E10BF88A0E2}"/>
     <hyperlink ref="K41" r:id="rId73" xr:uid="{0740A5E4-8C6B-4E30-A1C1-E1D4E4DE7981}"/>
+    <hyperlink ref="G42" r:id="rId74" xr:uid="{5F464448-B906-46DF-B4B6-33F79AFA8134}"/>
+    <hyperlink ref="K42" r:id="rId75" xr:uid="{E6CA8453-6C24-49A1-ACD9-1D25B10D7222}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId74"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId76"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
PLAU Folder clean user fi
git-tfs-id: [https://dev.azure.com/TR-Legal-Cobalt]$/Cobalt QED Testing/PLPlusANZ;C1228686
</commit_message>
<xml_diff>
--- a/PLPlusANZ-Tests/src/test/resources/CobaltUsers.xlsx
+++ b/PLPlusANZ-Tests/src/test/resources/CobaltUsers.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23801"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F525FF6-7CC7-4DAE-A05A-760356C8F6FB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9AB06B29-1955-44C2-94DA-4CFBB829EF45}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="10440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="239" uniqueCount="142">
   <si>
     <t>UserName</t>
   </si>
@@ -440,6 +440,12 @@
   </si>
   <si>
     <t>PLNewAUtestuser4@mailinator.com</t>
+  </si>
+  <si>
+    <t>PLANZtestuser20</t>
+  </si>
+  <si>
+    <t>PLANZtestuser20@mailinator.com</t>
   </si>
 </sst>
 </file>
@@ -908,11 +914,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L42"/>
+  <dimension ref="A1:L43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A33" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A37" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane xSplit="1" topLeftCell="F1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="H50" sqref="H50"/>
+      <selection pane="topRight" activeCell="G52" sqref="G52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1973,6 +1979,30 @@
       <c r="L42" s="4" t="s">
         <v>63</v>
       </c>
+    </row>
+    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A43" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="B43" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="C43" s="4"/>
+      <c r="D43" s="4"/>
+      <c r="E43" s="4"/>
+      <c r="F43" s="4"/>
+      <c r="G43" s="5" t="s">
+        <v>141</v>
+      </c>
+      <c r="H43" s="4"/>
+      <c r="I43" s="4"/>
+      <c r="J43" s="11" t="s">
+        <v>94</v>
+      </c>
+      <c r="K43" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="L43" s="4"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:L34" xr:uid="{46BB54A7-56CE-4320-A2E8-912A1AFF98E7}"/>
@@ -2052,9 +2082,12 @@
     <hyperlink ref="K41" r:id="rId73" xr:uid="{0740A5E4-8C6B-4E30-A1C1-E1D4E4DE7981}"/>
     <hyperlink ref="G42" r:id="rId74" xr:uid="{5F464448-B906-46DF-B4B6-33F79AFA8134}"/>
     <hyperlink ref="K42" r:id="rId75" xr:uid="{E6CA8453-6C24-49A1-ACD9-1D25B10D7222}"/>
+    <hyperlink ref="G43" r:id="rId76" xr:uid="{6BA274A6-AD6C-4033-8066-CE9DD39D486D}"/>
+    <hyperlink ref="B43" r:id="rId77" xr:uid="{45267BDD-EFE6-4F84-B9F1-C067B8C13CAC}"/>
+    <hyperlink ref="K43" r:id="rId78" xr:uid="{5DDE83B4-C370-46FC-8954-F1F874EB471F}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId76"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId79"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
PLAU Pros user fix
git-tfs-id: [https://dev.azure.com/TR-Legal-Cobalt]$/Cobalt QED Testing/PLPlusANZ;C1229599
</commit_message>
<xml_diff>
--- a/PLPlusANZ-Tests/src/test/resources/CobaltUsers.xlsx
+++ b/PLPlusANZ-Tests/src/test/resources/CobaltUsers.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23801"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9AB06B29-1955-44C2-94DA-4CFBB829EF45}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89DE177B-F167-4450-ACF1-FD34556E62B5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="10440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -391,9 +391,6 @@
     <t>P@ssword2</t>
   </si>
   <si>
-    <t>P@ssword4</t>
-  </si>
-  <si>
     <t>PLANZtestuser2</t>
   </si>
   <si>
@@ -446,6 +443,9 @@
   </si>
   <si>
     <t>PLANZtestuser20@mailinator.com</t>
+  </si>
+  <si>
+    <t>P@ssword5</t>
   </si>
 </sst>
 </file>
@@ -916,9 +916,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane xSplit="1" topLeftCell="F1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="G52" sqref="G52"/>
+      <selection pane="topRight" activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1321,7 +1321,7 @@
         <v>62</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>123</v>
+        <v>141</v>
       </c>
       <c r="C16" s="4"/>
       <c r="D16" s="4"/>
@@ -1784,7 +1784,7 @@
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A35" s="4" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B35" s="5" t="s">
         <v>122</v>
@@ -1794,7 +1794,7 @@
       <c r="E35" s="4"/>
       <c r="F35" s="4"/>
       <c r="G35" s="5" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="H35" s="4"/>
       <c r="I35" s="4"/>
@@ -1804,7 +1804,7 @@
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A36" s="4" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B36" s="5" t="s">
         <v>122</v>
@@ -1814,7 +1814,7 @@
       <c r="E36" s="4"/>
       <c r="F36" s="4"/>
       <c r="G36" s="5" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="H36" s="4"/>
       <c r="I36" s="4"/>
@@ -1830,7 +1830,7 @@
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A37" s="4" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B37" s="5" t="s">
         <v>122</v>
@@ -1840,7 +1840,7 @@
       <c r="E37" s="4"/>
       <c r="F37" s="4"/>
       <c r="G37" s="5" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="H37" s="4"/>
       <c r="I37" s="4"/>
@@ -1856,7 +1856,7 @@
     </row>
     <row r="38" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A38" s="4" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B38" s="5" t="s">
         <v>122</v>
@@ -1866,7 +1866,7 @@
       <c r="E38" s="4"/>
       <c r="F38" s="4"/>
       <c r="G38" s="5" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="H38" s="4"/>
       <c r="I38" s="4"/>
@@ -1880,7 +1880,7 @@
     </row>
     <row r="39" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A39" s="4" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B39" s="5" t="s">
         <v>122</v>
@@ -1890,7 +1890,7 @@
       <c r="E39" s="4"/>
       <c r="F39" s="4"/>
       <c r="G39" s="5" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="H39" s="4"/>
       <c r="I39" s="4"/>
@@ -1904,17 +1904,17 @@
     </row>
     <row r="40" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A40" s="4" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B40" s="5" t="s">
-        <v>123</v>
+        <v>141</v>
       </c>
       <c r="C40" s="4"/>
       <c r="D40" s="4"/>
       <c r="E40" s="4"/>
       <c r="F40" s="4"/>
       <c r="G40" s="5" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="H40" s="4"/>
       <c r="I40" s="4"/>
@@ -1930,17 +1930,17 @@
     </row>
     <row r="41" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A41" s="4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B41" s="5" t="s">
-        <v>123</v>
+        <v>141</v>
       </c>
       <c r="C41" s="4"/>
       <c r="D41" s="4"/>
       <c r="E41" s="4"/>
       <c r="F41" s="4"/>
       <c r="G41" s="5" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="H41" s="4"/>
       <c r="I41" s="4"/>
@@ -1956,7 +1956,7 @@
     </row>
     <row r="42" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A42" s="2" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B42" s="4" t="s">
         <v>122</v>
@@ -1966,7 +1966,7 @@
       <c r="E42" s="4"/>
       <c r="F42" s="4"/>
       <c r="G42" s="5" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="H42" s="4"/>
       <c r="I42" s="4"/>
@@ -1982,7 +1982,7 @@
     </row>
     <row r="43" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A43" s="2" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B43" s="5" t="s">
         <v>122</v>
@@ -1992,7 +1992,7 @@
       <c r="E43" s="4"/>
       <c r="F43" s="4"/>
       <c r="G43" s="5" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="H43" s="4"/>
       <c r="I43" s="4"/>

</xml_diff>

<commit_message>
PLAU folders clean user fix
git-tfs-id: [https://dev.azure.com/TR-Legal-Cobalt]$/Cobalt QED Testing/PLPlusANZ;C1230842
</commit_message>
<xml_diff>
--- a/PLPlusANZ-Tests/src/test/resources/CobaltUsers.xlsx
+++ b/PLPlusANZ-Tests/src/test/resources/CobaltUsers.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23801"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89DE177B-F167-4450-ACF1-FD34556E62B5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9EB5346-5D63-4524-A30D-1C81A2614018}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="10440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="239" uniqueCount="142">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="144">
   <si>
     <t>UserName</t>
   </si>
@@ -446,6 +446,12 @@
   </si>
   <si>
     <t>P@ssword5</t>
+  </si>
+  <si>
+    <t>PLANZFolderUser20</t>
+  </si>
+  <si>
+    <t>PLANZFolderUser20@mailinator.com</t>
   </si>
 </sst>
 </file>
@@ -914,11 +920,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L43"/>
+  <dimension ref="A1:L44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="F1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="I11" sqref="I11"/>
+    <sheetView tabSelected="1" topLeftCell="A32" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="C48" sqref="C48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2003,6 +2009,30 @@
         <v>108</v>
       </c>
       <c r="L43" s="4"/>
+    </row>
+    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A44" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="B44" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="C44" s="4"/>
+      <c r="D44" s="4"/>
+      <c r="E44" s="4"/>
+      <c r="F44" s="4"/>
+      <c r="G44" s="5" t="s">
+        <v>143</v>
+      </c>
+      <c r="H44" s="4"/>
+      <c r="I44" s="4"/>
+      <c r="J44" s="11" t="s">
+        <v>94</v>
+      </c>
+      <c r="K44" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="L44" s="4"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:L34" xr:uid="{46BB54A7-56CE-4320-A2E8-912A1AFF98E7}"/>
@@ -2085,9 +2115,12 @@
     <hyperlink ref="G43" r:id="rId76" xr:uid="{6BA274A6-AD6C-4033-8066-CE9DD39D486D}"/>
     <hyperlink ref="B43" r:id="rId77" xr:uid="{45267BDD-EFE6-4F84-B9F1-C067B8C13CAC}"/>
     <hyperlink ref="K43" r:id="rId78" xr:uid="{5DDE83B4-C370-46FC-8954-F1F874EB471F}"/>
+    <hyperlink ref="G44" r:id="rId79" xr:uid="{E4CD0F3F-5232-4201-86F5-AC70367C2A41}"/>
+    <hyperlink ref="B44" r:id="rId80" xr:uid="{C645C62B-924B-4902-B6D4-985325A1233E}"/>
+    <hyperlink ref="K44" r:id="rId81" xr:uid="{7C3E5A98-3D67-479C-A80A-CB226A1F15E2}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId79"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId82"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
VM - Annotations - updated the users
git-tfs-id: [https://dev.azure.com/TR-Legal-Cobalt]$/Cobalt QED Testing/PLPlusANZ;C1232820
</commit_message>
<xml_diff>
--- a/PLPlusANZ-Tests/src/test/resources/CobaltUsers.xlsx
+++ b/PLPlusANZ-Tests/src/test/resources/CobaltUsers.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23801"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9EB5346-5D63-4524-A30D-1C81A2614018}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77C5401A-AEC9-46DF-BEB1-7CDD671E25B5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="10440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-24120" yWindow="-6855" windowWidth="24240" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Users" sheetId="1" r:id="rId1"/>
@@ -922,9 +922,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A32" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A17" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="C48" sqref="C48"/>
+      <selection pane="topRight" activeCell="D37" sqref="D37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1726,8 +1726,8 @@
       <c r="A32" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="B32" s="4" t="s">
-        <v>13</v>
+      <c r="B32" s="5" t="s">
+        <v>122</v>
       </c>
       <c r="C32" s="4"/>
       <c r="D32" s="4"/>
@@ -2118,9 +2118,10 @@
     <hyperlink ref="G44" r:id="rId79" xr:uid="{E4CD0F3F-5232-4201-86F5-AC70367C2A41}"/>
     <hyperlink ref="B44" r:id="rId80" xr:uid="{C645C62B-924B-4902-B6D4-985325A1233E}"/>
     <hyperlink ref="K44" r:id="rId81" xr:uid="{7C3E5A98-3D67-479C-A80A-CB226A1F15E2}"/>
+    <hyperlink ref="B32" r:id="rId82" xr:uid="{649C10C0-9C1D-476C-963F-26F5B239BCFB}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId82"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId83"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
KM - PLAU - Annotations Suite Rebalancing
git-tfs-id: [https://dev.azure.com/TR-Legal-Cobalt]$/Cobalt QED Testing/PLPlusANZ;C1256679
</commit_message>
<xml_diff>
--- a/PLPlusANZ-Tests/src/test/resources/CobaltUsers.xlsx
+++ b/PLPlusANZ-Tests/src/test/resources/CobaltUsers.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24326"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D90D5714-B940-4A79-8BFC-DBFDC8D00BA2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1F81583-1757-4189-8904-D7DA60447DF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3030" yWindow="3030" windowWidth="17280" windowHeight="8955" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Users" sheetId="1" r:id="rId1"/>
@@ -13,14 +13,14 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Users!$A$1:$L$34</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Users!$A$1:$L$37</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="277" uniqueCount="160">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="292" uniqueCount="166">
   <si>
     <t>UserName</t>
   </si>
@@ -500,6 +500,24 @@
   </si>
   <si>
     <t>PLAUtestuser11@mailinator.com</t>
+  </si>
+  <si>
+    <t>auAnnotationUser4</t>
+  </si>
+  <si>
+    <t>auannotationuser4@mailinator.com</t>
+  </si>
+  <si>
+    <t>auAnnotationUser5</t>
+  </si>
+  <si>
+    <t>auannotationuser5@mailinator.com</t>
+  </si>
+  <si>
+    <t>auAnnotationUser6</t>
+  </si>
+  <si>
+    <t>auannotationuser6@mailinator.com</t>
   </si>
 </sst>
 </file>
@@ -968,11 +986,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L52"/>
+  <dimension ref="A1:L55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="E52" sqref="E52"/>
+      <selection pane="topRight" activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1772,9 +1790,9 @@
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="B32" s="5" t="s">
+        <v>160</v>
+      </c>
+      <c r="B32" s="4" t="s">
         <v>122</v>
       </c>
       <c r="C32" s="4"/>
@@ -1784,20 +1802,22 @@
       </c>
       <c r="F32" s="4"/>
       <c r="G32" s="9" t="s">
-        <v>48</v>
+        <v>161</v>
       </c>
       <c r="H32" s="5"/>
       <c r="I32" s="5"/>
       <c r="J32" s="5"/>
       <c r="K32" s="5"/>
-      <c r="L32" s="4"/>
+      <c r="L32" s="4" t="s">
+        <v>63</v>
+      </c>
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
-        <v>49</v>
+        <v>162</v>
       </c>
       <c r="B33" s="4" t="s">
-        <v>13</v>
+        <v>122</v>
       </c>
       <c r="C33" s="4"/>
       <c r="D33" s="4"/>
@@ -1806,111 +1826,109 @@
       </c>
       <c r="F33" s="4"/>
       <c r="G33" s="9" t="s">
-        <v>50</v>
+        <v>163</v>
       </c>
       <c r="H33" s="5"/>
       <c r="I33" s="5"/>
       <c r="J33" s="5"/>
       <c r="K33" s="5"/>
-      <c r="L33" s="4"/>
+      <c r="L33" s="4" t="s">
+        <v>63</v>
+      </c>
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A34" s="16" t="s">
-        <v>51</v>
-      </c>
-      <c r="B34" s="13" t="s">
-        <v>13</v>
-      </c>
-      <c r="C34" s="13"/>
-      <c r="D34" s="13"/>
-      <c r="E34" s="13" t="s">
+      <c r="A34" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="B34" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="C34" s="4"/>
+      <c r="D34" s="4"/>
+      <c r="E34" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="F34" s="13"/>
-      <c r="G34" s="17" t="s">
-        <v>52</v>
-      </c>
-      <c r="H34" s="12"/>
-      <c r="I34" s="12"/>
-      <c r="J34" s="12"/>
-      <c r="K34" s="12"/>
-      <c r="L34" s="13"/>
+      <c r="F34" s="4"/>
+      <c r="G34" s="9" t="s">
+        <v>165</v>
+      </c>
+      <c r="H34" s="5"/>
+      <c r="I34" s="5"/>
+      <c r="J34" s="5"/>
+      <c r="K34" s="5"/>
+      <c r="L34" s="4" t="s">
+        <v>63</v>
+      </c>
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A35" s="4" t="s">
-        <v>123</v>
+      <c r="A35" s="2" t="s">
+        <v>47</v>
       </c>
       <c r="B35" s="5" t="s">
         <v>122</v>
       </c>
       <c r="C35" s="4"/>
       <c r="D35" s="4"/>
-      <c r="E35" s="4"/>
+      <c r="E35" s="4" t="s">
+        <v>45</v>
+      </c>
       <c r="F35" s="4"/>
-      <c r="G35" s="5" t="s">
-        <v>124</v>
-      </c>
-      <c r="H35" s="4"/>
-      <c r="I35" s="4"/>
-      <c r="J35" s="4"/>
-      <c r="K35" s="4"/>
+      <c r="G35" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="H35" s="5"/>
+      <c r="I35" s="5"/>
+      <c r="J35" s="5"/>
+      <c r="K35" s="5"/>
       <c r="L35" s="4"/>
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A36" s="4" t="s">
-        <v>127</v>
-      </c>
-      <c r="B36" s="5" t="s">
-        <v>122</v>
+      <c r="A36" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B36" s="4" t="s">
+        <v>13</v>
       </c>
       <c r="C36" s="4"/>
       <c r="D36" s="4"/>
-      <c r="E36" s="4"/>
+      <c r="E36" s="4" t="s">
+        <v>45</v>
+      </c>
       <c r="F36" s="4"/>
-      <c r="G36" s="5" t="s">
-        <v>129</v>
-      </c>
-      <c r="H36" s="4"/>
-      <c r="I36" s="4"/>
-      <c r="J36" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="K36" s="5" t="s">
-        <v>119</v>
-      </c>
-      <c r="L36" s="4" t="s">
-        <v>63</v>
-      </c>
+      <c r="G36" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="H36" s="5"/>
+      <c r="I36" s="5"/>
+      <c r="J36" s="5"/>
+      <c r="K36" s="5"/>
+      <c r="L36" s="4"/>
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A37" s="4" t="s">
-        <v>128</v>
-      </c>
-      <c r="B37" s="5" t="s">
-        <v>122</v>
-      </c>
-      <c r="C37" s="4"/>
-      <c r="D37" s="4"/>
-      <c r="E37" s="4"/>
-      <c r="F37" s="4"/>
-      <c r="G37" s="5" t="s">
-        <v>130</v>
-      </c>
-      <c r="H37" s="4"/>
-      <c r="I37" s="4"/>
-      <c r="J37" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="K37" s="5" t="s">
-        <v>119</v>
-      </c>
-      <c r="L37" s="4" t="s">
-        <v>63</v>
-      </c>
+      <c r="A37" s="16" t="s">
+        <v>51</v>
+      </c>
+      <c r="B37" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="C37" s="13"/>
+      <c r="D37" s="13"/>
+      <c r="E37" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="F37" s="13"/>
+      <c r="G37" s="17" t="s">
+        <v>52</v>
+      </c>
+      <c r="H37" s="12"/>
+      <c r="I37" s="12"/>
+      <c r="J37" s="12"/>
+      <c r="K37" s="12"/>
+      <c r="L37" s="13"/>
     </row>
     <row r="38" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A38" s="4" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="B38" s="5" t="s">
         <v>122</v>
@@ -1920,21 +1938,17 @@
       <c r="E38" s="4"/>
       <c r="F38" s="4"/>
       <c r="G38" s="5" t="s">
-        <v>131</v>
+        <v>124</v>
       </c>
       <c r="H38" s="4"/>
       <c r="I38" s="4"/>
-      <c r="J38" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="K38" s="5" t="s">
-        <v>118</v>
-      </c>
+      <c r="J38" s="4"/>
+      <c r="K38" s="4"/>
       <c r="L38" s="4"/>
     </row>
     <row r="39" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A39" s="4" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="B39" s="5" t="s">
         <v>122</v>
@@ -1944,39 +1958,41 @@
       <c r="E39" s="4"/>
       <c r="F39" s="4"/>
       <c r="G39" s="5" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="H39" s="4"/>
       <c r="I39" s="4"/>
       <c r="J39" s="2" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="K39" s="5" t="s">
-        <v>118</v>
-      </c>
-      <c r="L39" s="4"/>
+        <v>119</v>
+      </c>
+      <c r="L39" s="4" t="s">
+        <v>63</v>
+      </c>
     </row>
     <row r="40" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A40" s="4" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="B40" s="5" t="s">
-        <v>141</v>
+        <v>122</v>
       </c>
       <c r="C40" s="4"/>
       <c r="D40" s="4"/>
       <c r="E40" s="4"/>
       <c r="F40" s="4"/>
       <c r="G40" s="5" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="H40" s="4"/>
       <c r="I40" s="4"/>
       <c r="J40" s="2" t="s">
-        <v>96</v>
+        <v>105</v>
       </c>
       <c r="K40" s="5" t="s">
-        <v>110</v>
+        <v>119</v>
       </c>
       <c r="L40" s="4" t="s">
         <v>63</v>
@@ -1984,35 +2000,33 @@
     </row>
     <row r="41" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A41" s="4" t="s">
-        <v>134</v>
+        <v>125</v>
       </c>
       <c r="B41" s="5" t="s">
-        <v>141</v>
+        <v>122</v>
       </c>
       <c r="C41" s="4"/>
       <c r="D41" s="4"/>
       <c r="E41" s="4"/>
       <c r="F41" s="4"/>
       <c r="G41" s="5" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="H41" s="4"/>
       <c r="I41" s="4"/>
       <c r="J41" s="2" t="s">
-        <v>96</v>
+        <v>104</v>
       </c>
       <c r="K41" s="5" t="s">
-        <v>110</v>
-      </c>
-      <c r="L41" s="4" t="s">
-        <v>63</v>
-      </c>
+        <v>118</v>
+      </c>
+      <c r="L41" s="4"/>
     </row>
     <row r="42" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A42" s="2" t="s">
-        <v>137</v>
-      </c>
-      <c r="B42" s="4" t="s">
+      <c r="A42" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="B42" s="5" t="s">
         <v>122</v>
       </c>
       <c r="C42" s="4"/>
@@ -2020,73 +2034,75 @@
       <c r="E42" s="4"/>
       <c r="F42" s="4"/>
       <c r="G42" s="5" t="s">
-        <v>138</v>
+        <v>132</v>
       </c>
       <c r="H42" s="4"/>
       <c r="I42" s="4"/>
       <c r="J42" s="2" t="s">
-        <v>97</v>
+        <v>104</v>
       </c>
       <c r="K42" s="5" t="s">
-        <v>111</v>
-      </c>
-      <c r="L42" s="4" t="s">
-        <v>63</v>
-      </c>
+        <v>118</v>
+      </c>
+      <c r="L42" s="4"/>
     </row>
     <row r="43" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A43" s="2" t="s">
-        <v>139</v>
+      <c r="A43" s="4" t="s">
+        <v>133</v>
       </c>
       <c r="B43" s="5" t="s">
-        <v>122</v>
+        <v>141</v>
       </c>
       <c r="C43" s="4"/>
       <c r="D43" s="4"/>
       <c r="E43" s="4"/>
       <c r="F43" s="4"/>
       <c r="G43" s="5" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="H43" s="4"/>
       <c r="I43" s="4"/>
-      <c r="J43" s="11" t="s">
-        <v>94</v>
+      <c r="J43" s="2" t="s">
+        <v>96</v>
       </c>
       <c r="K43" s="5" t="s">
-        <v>108</v>
-      </c>
-      <c r="L43" s="4"/>
+        <v>110</v>
+      </c>
+      <c r="L43" s="4" t="s">
+        <v>63</v>
+      </c>
     </row>
     <row r="44" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A44" s="2" t="s">
-        <v>142</v>
+      <c r="A44" s="4" t="s">
+        <v>134</v>
       </c>
       <c r="B44" s="5" t="s">
-        <v>122</v>
+        <v>141</v>
       </c>
       <c r="C44" s="4"/>
       <c r="D44" s="4"/>
       <c r="E44" s="4"/>
       <c r="F44" s="4"/>
       <c r="G44" s="5" t="s">
-        <v>143</v>
+        <v>136</v>
       </c>
       <c r="H44" s="4"/>
       <c r="I44" s="4"/>
-      <c r="J44" s="11" t="s">
-        <v>94</v>
+      <c r="J44" s="2" t="s">
+        <v>96</v>
       </c>
       <c r="K44" s="5" t="s">
-        <v>108</v>
-      </c>
-      <c r="L44" s="4"/>
+        <v>110</v>
+      </c>
+      <c r="L44" s="4" t="s">
+        <v>63</v>
+      </c>
     </row>
     <row r="45" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A45" s="2" t="s">
-        <v>144</v>
-      </c>
-      <c r="B45" s="5" t="s">
+        <v>137</v>
+      </c>
+      <c r="B45" s="4" t="s">
         <v>122</v>
       </c>
       <c r="C45" s="4"/>
@@ -2094,19 +2110,23 @@
       <c r="E45" s="4"/>
       <c r="F45" s="4"/>
       <c r="G45" s="5" t="s">
-        <v>150</v>
+        <v>138</v>
       </c>
       <c r="H45" s="4"/>
       <c r="I45" s="4"/>
-      <c r="J45" s="11"/>
-      <c r="K45" s="5"/>
+      <c r="J45" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="K45" s="5" t="s">
+        <v>111</v>
+      </c>
       <c r="L45" s="4" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="46" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A46" s="2" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="B46" s="5" t="s">
         <v>122</v>
@@ -2116,19 +2136,21 @@
       <c r="E46" s="4"/>
       <c r="F46" s="4"/>
       <c r="G46" s="5" t="s">
-        <v>151</v>
+        <v>140</v>
       </c>
       <c r="H46" s="4"/>
       <c r="I46" s="4"/>
-      <c r="J46" s="11"/>
-      <c r="K46" s="5"/>
-      <c r="L46" s="4" t="s">
-        <v>63</v>
-      </c>
+      <c r="J46" s="11" t="s">
+        <v>94</v>
+      </c>
+      <c r="K46" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="L46" s="4"/>
     </row>
     <row r="47" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A47" s="2" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="B47" s="5" t="s">
         <v>122</v>
@@ -2138,19 +2160,21 @@
       <c r="E47" s="4"/>
       <c r="F47" s="4"/>
       <c r="G47" s="5" t="s">
-        <v>152</v>
+        <v>143</v>
       </c>
       <c r="H47" s="4"/>
       <c r="I47" s="4"/>
-      <c r="J47" s="11"/>
-      <c r="K47" s="5"/>
-      <c r="L47" s="4" t="s">
-        <v>63</v>
-      </c>
+      <c r="J47" s="11" t="s">
+        <v>94</v>
+      </c>
+      <c r="K47" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="L47" s="4"/>
     </row>
     <row r="48" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A48" s="2" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="B48" s="5" t="s">
         <v>122</v>
@@ -2160,7 +2184,7 @@
       <c r="E48" s="4"/>
       <c r="F48" s="4"/>
       <c r="G48" s="5" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="H48" s="4"/>
       <c r="I48" s="4"/>
@@ -2172,7 +2196,7 @@
     </row>
     <row r="49" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A49" s="2" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="B49" s="5" t="s">
         <v>122</v>
@@ -2182,7 +2206,7 @@
       <c r="E49" s="4"/>
       <c r="F49" s="4"/>
       <c r="G49" s="5" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="H49" s="4"/>
       <c r="I49" s="4"/>
@@ -2194,7 +2218,7 @@
     </row>
     <row r="50" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A50" s="2" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="B50" s="5" t="s">
         <v>122</v>
@@ -2204,23 +2228,19 @@
       <c r="E50" s="4"/>
       <c r="F50" s="4"/>
       <c r="G50" s="5" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="H50" s="4"/>
       <c r="I50" s="4"/>
-      <c r="J50" s="11" t="s">
-        <v>94</v>
-      </c>
-      <c r="K50" s="5" t="s">
-        <v>108</v>
-      </c>
+      <c r="J50" s="11"/>
+      <c r="K50" s="5"/>
       <c r="L50" s="4" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="51" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A51" s="2" t="s">
-        <v>156</v>
+        <v>147</v>
       </c>
       <c r="B51" s="5" t="s">
         <v>122</v>
@@ -2230,7 +2250,7 @@
       <c r="E51" s="4"/>
       <c r="F51" s="4"/>
       <c r="G51" s="5" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="H51" s="4"/>
       <c r="I51" s="4"/>
@@ -2242,24 +2262,94 @@
     </row>
     <row r="52" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A52" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="B52" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="C52" s="4"/>
+      <c r="D52" s="4"/>
+      <c r="E52" s="4"/>
+      <c r="F52" s="4"/>
+      <c r="G52" s="5" t="s">
+        <v>154</v>
+      </c>
+      <c r="H52" s="4"/>
+      <c r="I52" s="4"/>
+      <c r="J52" s="11"/>
+      <c r="K52" s="5"/>
+      <c r="L52" s="4" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="53" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A53" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="B53" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="C53" s="4"/>
+      <c r="D53" s="4"/>
+      <c r="E53" s="4"/>
+      <c r="F53" s="4"/>
+      <c r="G53" s="5" t="s">
+        <v>155</v>
+      </c>
+      <c r="H53" s="4"/>
+      <c r="I53" s="4"/>
+      <c r="J53" s="11" t="s">
+        <v>94</v>
+      </c>
+      <c r="K53" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="L53" s="4" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="54" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A54" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="B54" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="C54" s="4"/>
+      <c r="D54" s="4"/>
+      <c r="E54" s="4"/>
+      <c r="F54" s="4"/>
+      <c r="G54" s="5" t="s">
+        <v>157</v>
+      </c>
+      <c r="H54" s="4"/>
+      <c r="I54" s="4"/>
+      <c r="J54" s="11"/>
+      <c r="K54" s="5"/>
+      <c r="L54" s="4" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="55" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A55" s="2" t="s">
         <v>158</v>
       </c>
-      <c r="B52" s="5" t="s">
-        <v>122</v>
-      </c>
-      <c r="G52" s="5" t="s">
+      <c r="B55" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="G55" s="5" t="s">
         <v>159</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:L34" xr:uid="{46BB54A7-56CE-4320-A2E8-912A1AFF98E7}"/>
+  <autoFilter ref="A1:L37" xr:uid="{46BB54A7-56CE-4320-A2E8-912A1AFF98E7}"/>
   <hyperlinks>
     <hyperlink ref="G3" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
     <hyperlink ref="G4" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
     <hyperlink ref="G6" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
     <hyperlink ref="G7" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
-    <hyperlink ref="G32" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
-    <hyperlink ref="G33" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="G35" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="G36" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
     <hyperlink ref="G30" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
     <hyperlink ref="G31" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
     <hyperlink ref="G14" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
@@ -2308,51 +2398,51 @@
     <hyperlink ref="B26" r:id="rId52" xr:uid="{5A9A556E-193D-4906-BD07-952EF6BF8A37}"/>
     <hyperlink ref="B29" r:id="rId53" xr:uid="{DBE6C47B-31D5-4908-8C16-D56DABF274BE}"/>
     <hyperlink ref="B30" r:id="rId54" xr:uid="{3812BCE2-3A74-426B-B41D-3AFE6E7BDADB}"/>
-    <hyperlink ref="B35" r:id="rId55" xr:uid="{F9CEA64B-443C-4110-8FE5-4820AD15E535}"/>
-    <hyperlink ref="G35" r:id="rId56" xr:uid="{AF615813-6EF6-4298-A920-CB3FCA725BE7}"/>
-    <hyperlink ref="B38" r:id="rId57" xr:uid="{89F25A13-A172-497F-8CE3-5D4409F41B4F}"/>
-    <hyperlink ref="B39" r:id="rId58" xr:uid="{24E87864-B135-49BA-BE62-962A47FCE58C}"/>
-    <hyperlink ref="K38" r:id="rId59" xr:uid="{40477EF3-2B66-4270-8235-D256CBAB4BBF}"/>
-    <hyperlink ref="K39" r:id="rId60" xr:uid="{BAD7E65A-8416-4F76-AE1C-2B21061C4463}"/>
-    <hyperlink ref="B36" r:id="rId61" xr:uid="{6D23639B-B2F3-48A4-A5D8-C0C4999D4D92}"/>
-    <hyperlink ref="K36" r:id="rId62" xr:uid="{4586EFD4-4608-4D09-9B23-192D12EE1FDF}"/>
-    <hyperlink ref="K37" r:id="rId63" xr:uid="{F37A5A5A-E6D6-45C7-9B40-0E4C7A81FDF0}"/>
-    <hyperlink ref="G36" r:id="rId64" xr:uid="{044F65C8-9B95-454E-8FD5-518DDDB9FB9B}"/>
-    <hyperlink ref="G37" r:id="rId65" xr:uid="{C953582D-F248-41C5-AC5B-A2EFB1FDA5EB}"/>
-    <hyperlink ref="G38" r:id="rId66" xr:uid="{6BC6EE1B-7E5F-4759-AA23-CEFF794BE365}"/>
-    <hyperlink ref="G39" r:id="rId67" xr:uid="{FA510CBE-0B1E-4C43-83D2-CE5F63427358}"/>
-    <hyperlink ref="B40" r:id="rId68" xr:uid="{E30FCD2F-28D5-472A-828D-370C1C5BEB7E}"/>
-    <hyperlink ref="B41" r:id="rId69" xr:uid="{F1B8F9CA-7DE9-46CE-BBA1-E7553E7DCDB1}"/>
-    <hyperlink ref="G40" r:id="rId70" xr:uid="{92DBAF28-DCED-4F04-BECB-34A8DC3BA4C5}"/>
-    <hyperlink ref="G41" r:id="rId71" xr:uid="{2E0446EE-618A-454A-9D8B-4B27BD2F86DA}"/>
-    <hyperlink ref="K40" r:id="rId72" xr:uid="{16F44302-BF74-4A5B-90C5-1E10BF88A0E2}"/>
-    <hyperlink ref="K41" r:id="rId73" xr:uid="{0740A5E4-8C6B-4E30-A1C1-E1D4E4DE7981}"/>
-    <hyperlink ref="G42" r:id="rId74" xr:uid="{5F464448-B906-46DF-B4B6-33F79AFA8134}"/>
-    <hyperlink ref="K42" r:id="rId75" xr:uid="{E6CA8453-6C24-49A1-ACD9-1D25B10D7222}"/>
-    <hyperlink ref="G43" r:id="rId76" xr:uid="{6BA274A6-AD6C-4033-8066-CE9DD39D486D}"/>
-    <hyperlink ref="B43" r:id="rId77" xr:uid="{45267BDD-EFE6-4F84-B9F1-C067B8C13CAC}"/>
-    <hyperlink ref="K43" r:id="rId78" xr:uid="{5DDE83B4-C370-46FC-8954-F1F874EB471F}"/>
-    <hyperlink ref="G44" r:id="rId79" xr:uid="{E4CD0F3F-5232-4201-86F5-AC70367C2A41}"/>
-    <hyperlink ref="B44" r:id="rId80" xr:uid="{C645C62B-924B-4902-B6D4-985325A1233E}"/>
-    <hyperlink ref="K44" r:id="rId81" xr:uid="{7C3E5A98-3D67-479C-A80A-CB226A1F15E2}"/>
-    <hyperlink ref="B32" r:id="rId82" xr:uid="{649C10C0-9C1D-476C-963F-26F5B239BCFB}"/>
-    <hyperlink ref="B45" r:id="rId83" xr:uid="{3B47E0B4-064C-424C-954C-8FDE30BEBCC6}"/>
-    <hyperlink ref="B46" r:id="rId84" xr:uid="{795E655C-F6DC-481B-9579-43EB73FC707B}"/>
-    <hyperlink ref="B47" r:id="rId85" xr:uid="{7DA48CE9-0A00-4BD3-AC77-B4F65DF1A4B9}"/>
-    <hyperlink ref="B48" r:id="rId86" xr:uid="{E57CD4AC-A045-4179-B6B2-58C26F1ADA62}"/>
-    <hyperlink ref="B49" r:id="rId87" xr:uid="{94ACDBD4-3E6E-4B1A-9862-0DAB814A65AB}"/>
-    <hyperlink ref="B50" r:id="rId88" xr:uid="{72D09C23-ACD5-43A5-B4B2-C9F7D693F424}"/>
-    <hyperlink ref="G45" r:id="rId89" xr:uid="{45D9945D-400B-4F59-89DB-86F442853353}"/>
-    <hyperlink ref="G46" r:id="rId90" xr:uid="{288C64BB-5DC1-48DD-91EC-9244A16EC44C}"/>
-    <hyperlink ref="G47" r:id="rId91" xr:uid="{BE79538B-2F89-477B-9B0D-AA2952D29675}"/>
-    <hyperlink ref="G48" r:id="rId92" xr:uid="{3A3C2B43-F93B-45FC-B80C-CB93C6481BB8}"/>
-    <hyperlink ref="G49" r:id="rId93" display="PLAUtestuser6@mailinator.com" xr:uid="{4EF71BBC-EDEB-4B9B-A160-452A348703D0}"/>
-    <hyperlink ref="G50" r:id="rId94" display="PLAUtestuser7@mailinator.com" xr:uid="{45B7E063-4022-4FE8-BD38-EAE8C38FA7ED}"/>
-    <hyperlink ref="K50" r:id="rId95" xr:uid="{6C269F0A-2EE2-4F54-BC10-699F4DC52C23}"/>
-    <hyperlink ref="B51" r:id="rId96" xr:uid="{209E1511-9F36-45EA-B6C5-EE74D938B54D}"/>
-    <hyperlink ref="G51" r:id="rId97" xr:uid="{9D42DA86-2677-4AB2-8455-5681E815217E}"/>
-    <hyperlink ref="B52" r:id="rId98" xr:uid="{A5A3377D-A990-4617-B025-F0B381234F89}"/>
-    <hyperlink ref="G52" r:id="rId99" xr:uid="{7167A2F3-6711-45BE-BC0F-E0CC2EF3991D}"/>
+    <hyperlink ref="B38" r:id="rId55" xr:uid="{F9CEA64B-443C-4110-8FE5-4820AD15E535}"/>
+    <hyperlink ref="G38" r:id="rId56" xr:uid="{AF615813-6EF6-4298-A920-CB3FCA725BE7}"/>
+    <hyperlink ref="B41" r:id="rId57" xr:uid="{89F25A13-A172-497F-8CE3-5D4409F41B4F}"/>
+    <hyperlink ref="B42" r:id="rId58" xr:uid="{24E87864-B135-49BA-BE62-962A47FCE58C}"/>
+    <hyperlink ref="K41" r:id="rId59" xr:uid="{40477EF3-2B66-4270-8235-D256CBAB4BBF}"/>
+    <hyperlink ref="K42" r:id="rId60" xr:uid="{BAD7E65A-8416-4F76-AE1C-2B21061C4463}"/>
+    <hyperlink ref="B39" r:id="rId61" xr:uid="{6D23639B-B2F3-48A4-A5D8-C0C4999D4D92}"/>
+    <hyperlink ref="K39" r:id="rId62" xr:uid="{4586EFD4-4608-4D09-9B23-192D12EE1FDF}"/>
+    <hyperlink ref="K40" r:id="rId63" xr:uid="{F37A5A5A-E6D6-45C7-9B40-0E4C7A81FDF0}"/>
+    <hyperlink ref="G39" r:id="rId64" xr:uid="{044F65C8-9B95-454E-8FD5-518DDDB9FB9B}"/>
+    <hyperlink ref="G40" r:id="rId65" xr:uid="{C953582D-F248-41C5-AC5B-A2EFB1FDA5EB}"/>
+    <hyperlink ref="G41" r:id="rId66" xr:uid="{6BC6EE1B-7E5F-4759-AA23-CEFF794BE365}"/>
+    <hyperlink ref="G42" r:id="rId67" xr:uid="{FA510CBE-0B1E-4C43-83D2-CE5F63427358}"/>
+    <hyperlink ref="B43" r:id="rId68" xr:uid="{E30FCD2F-28D5-472A-828D-370C1C5BEB7E}"/>
+    <hyperlink ref="B44" r:id="rId69" xr:uid="{F1B8F9CA-7DE9-46CE-BBA1-E7553E7DCDB1}"/>
+    <hyperlink ref="G43" r:id="rId70" xr:uid="{92DBAF28-DCED-4F04-BECB-34A8DC3BA4C5}"/>
+    <hyperlink ref="G44" r:id="rId71" xr:uid="{2E0446EE-618A-454A-9D8B-4B27BD2F86DA}"/>
+    <hyperlink ref="K43" r:id="rId72" xr:uid="{16F44302-BF74-4A5B-90C5-1E10BF88A0E2}"/>
+    <hyperlink ref="K44" r:id="rId73" xr:uid="{0740A5E4-8C6B-4E30-A1C1-E1D4E4DE7981}"/>
+    <hyperlink ref="G45" r:id="rId74" xr:uid="{5F464448-B906-46DF-B4B6-33F79AFA8134}"/>
+    <hyperlink ref="K45" r:id="rId75" xr:uid="{E6CA8453-6C24-49A1-ACD9-1D25B10D7222}"/>
+    <hyperlink ref="G46" r:id="rId76" xr:uid="{6BA274A6-AD6C-4033-8066-CE9DD39D486D}"/>
+    <hyperlink ref="B46" r:id="rId77" xr:uid="{45267BDD-EFE6-4F84-B9F1-C067B8C13CAC}"/>
+    <hyperlink ref="K46" r:id="rId78" xr:uid="{5DDE83B4-C370-46FC-8954-F1F874EB471F}"/>
+    <hyperlink ref="G47" r:id="rId79" xr:uid="{E4CD0F3F-5232-4201-86F5-AC70367C2A41}"/>
+    <hyperlink ref="B47" r:id="rId80" xr:uid="{C645C62B-924B-4902-B6D4-985325A1233E}"/>
+    <hyperlink ref="K47" r:id="rId81" xr:uid="{7C3E5A98-3D67-479C-A80A-CB226A1F15E2}"/>
+    <hyperlink ref="B35" r:id="rId82" xr:uid="{649C10C0-9C1D-476C-963F-26F5B239BCFB}"/>
+    <hyperlink ref="B48" r:id="rId83" xr:uid="{3B47E0B4-064C-424C-954C-8FDE30BEBCC6}"/>
+    <hyperlink ref="B49" r:id="rId84" xr:uid="{795E655C-F6DC-481B-9579-43EB73FC707B}"/>
+    <hyperlink ref="B50" r:id="rId85" xr:uid="{7DA48CE9-0A00-4BD3-AC77-B4F65DF1A4B9}"/>
+    <hyperlink ref="B51" r:id="rId86" xr:uid="{E57CD4AC-A045-4179-B6B2-58C26F1ADA62}"/>
+    <hyperlink ref="B52" r:id="rId87" xr:uid="{94ACDBD4-3E6E-4B1A-9862-0DAB814A65AB}"/>
+    <hyperlink ref="B53" r:id="rId88" xr:uid="{72D09C23-ACD5-43A5-B4B2-C9F7D693F424}"/>
+    <hyperlink ref="G48" r:id="rId89" xr:uid="{45D9945D-400B-4F59-89DB-86F442853353}"/>
+    <hyperlink ref="G49" r:id="rId90" xr:uid="{288C64BB-5DC1-48DD-91EC-9244A16EC44C}"/>
+    <hyperlink ref="G50" r:id="rId91" xr:uid="{BE79538B-2F89-477B-9B0D-AA2952D29675}"/>
+    <hyperlink ref="G51" r:id="rId92" xr:uid="{3A3C2B43-F93B-45FC-B80C-CB93C6481BB8}"/>
+    <hyperlink ref="G52" r:id="rId93" display="PLAUtestuser6@mailinator.com" xr:uid="{4EF71BBC-EDEB-4B9B-A160-452A348703D0}"/>
+    <hyperlink ref="G53" r:id="rId94" display="PLAUtestuser7@mailinator.com" xr:uid="{45B7E063-4022-4FE8-BD38-EAE8C38FA7ED}"/>
+    <hyperlink ref="K53" r:id="rId95" xr:uid="{6C269F0A-2EE2-4F54-BC10-699F4DC52C23}"/>
+    <hyperlink ref="B54" r:id="rId96" xr:uid="{209E1511-9F36-45EA-B6C5-EE74D938B54D}"/>
+    <hyperlink ref="G54" r:id="rId97" xr:uid="{9D42DA86-2677-4AB2-8455-5681E815217E}"/>
+    <hyperlink ref="B55" r:id="rId98" xr:uid="{A5A3377D-A990-4617-B025-F0B381234F89}"/>
+    <hyperlink ref="G55" r:id="rId99" xr:uid="{7167A2F3-6711-45BE-BC0F-E0CC2EF3991D}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId100"/>

</xml_diff>

<commit_message>
SA-PLAU-Delivery Suite Prod users fix
git-tfs-id: [https://dev.azure.com/TR-Legal-Cobalt]$/Cobalt QED Testing/PLPlusANZ;C1258320
</commit_message>
<xml_diff>
--- a/PLPlusANZ-Tests/src/test/resources/CobaltUsers.xlsx
+++ b/PLPlusANZ-Tests/src/test/resources/CobaltUsers.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24326"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1F81583-1757-4189-8904-D7DA60447DF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BA6DCAE-520B-4605-B018-242AAA9E2A5E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3030" yWindow="3030" windowWidth="17280" windowHeight="8955" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Users" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="292" uniqueCount="166">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="296" uniqueCount="166">
   <si>
     <t>UserName</t>
   </si>
@@ -990,7 +990,7 @@
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A25" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="C32" sqref="C32"/>
+      <selection pane="topRight" activeCell="A45" sqref="A45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2188,8 +2188,12 @@
       </c>
       <c r="H48" s="4"/>
       <c r="I48" s="4"/>
-      <c r="J48" s="11"/>
-      <c r="K48" s="5"/>
+      <c r="J48" s="11" t="s">
+        <v>97</v>
+      </c>
+      <c r="K48" s="5" t="s">
+        <v>111</v>
+      </c>
       <c r="L48" s="4" t="s">
         <v>63</v>
       </c>
@@ -2232,8 +2236,12 @@
       </c>
       <c r="H50" s="4"/>
       <c r="I50" s="4"/>
-      <c r="J50" s="11"/>
-      <c r="K50" s="5"/>
+      <c r="J50" s="11" t="s">
+        <v>97</v>
+      </c>
+      <c r="K50" s="5" t="s">
+        <v>111</v>
+      </c>
       <c r="L50" s="4" t="s">
         <v>63</v>
       </c>
@@ -2443,9 +2451,11 @@
     <hyperlink ref="G54" r:id="rId97" xr:uid="{9D42DA86-2677-4AB2-8455-5681E815217E}"/>
     <hyperlink ref="B55" r:id="rId98" xr:uid="{A5A3377D-A990-4617-B025-F0B381234F89}"/>
     <hyperlink ref="G55" r:id="rId99" xr:uid="{7167A2F3-6711-45BE-BC0F-E0CC2EF3991D}"/>
+    <hyperlink ref="K48" r:id="rId100" xr:uid="{BB0D1967-6F53-4874-A6AF-8F4F2D49ED7C}"/>
+    <hyperlink ref="K50" r:id="rId101" xr:uid="{4B235659-962D-4EA1-8559-61402EAF4D67}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId100"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId102"/>
 </worksheet>
 </file>
 

</xml_diff>